<commit_message>
Data Envelopemnt Analysis For One Input And Two Output
</commit_message>
<xml_diff>
--- a/DataEnvelopmentAnalysisOneInputAndTwoOutput.xlsx
+++ b/DataEnvelopmentAnalysisOneInputAndTwoOutput.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Lp1" sheetId="1" r:id="rId1"/>
@@ -185,7 +185,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="27">
   <si>
     <t xml:space="preserve">Input </t>
   </si>
@@ -230,6 +230,42 @@
   </si>
   <si>
     <t>&lt;=</t>
+  </si>
+  <si>
+    <t>y12</t>
+  </si>
+  <si>
+    <t>y22</t>
+  </si>
+  <si>
+    <t>y13</t>
+  </si>
+  <si>
+    <t>y23</t>
+  </si>
+  <si>
+    <t>y14</t>
+  </si>
+  <si>
+    <t>y24</t>
+  </si>
+  <si>
+    <t>y15</t>
+  </si>
+  <si>
+    <t>y25</t>
+  </si>
+  <si>
+    <t>x12</t>
+  </si>
+  <si>
+    <t>x13</t>
+  </si>
+  <si>
+    <t>x14</t>
+  </si>
+  <si>
+    <t>x15</t>
   </si>
 </sst>
 </file>
@@ -573,7 +609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -786,7 +822,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="A1:XFD1048576"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -830,13 +866,13 @@
         <v>15</v>
       </c>
       <c r="I4" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="J4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="K4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -998,7 +1034,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="A1:XFD1048576"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1042,13 +1078,13 @@
         <v>15</v>
       </c>
       <c r="I4" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="J4" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="K4" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -1210,7 +1246,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1254,13 +1290,13 @@
         <v>15</v>
       </c>
       <c r="I4" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="J4" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="K4" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -1421,8 +1457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1466,13 +1502,13 @@
         <v>15</v>
       </c>
       <c r="I4" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="J4" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="K4" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">

</xml_diff>